<commit_message>
Correcting calibration value for plant dry aboveground biomass
</commit_message>
<xml_diff>
--- a/rawdata/PastureMeterCalibration.xlsx
+++ b/rawdata/PastureMeterCalibration.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elwel\OneDrive\Desktop\Smithsonian\Field2022\rawData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elwel\OneDrive\Desktop\AppraisingGrazing\rawdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B238E667-761F-461A-84A4-71360BB96DBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC2A634D-E466-421B-B1B7-B0D11EA19BD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{529C1CFA-C348-486F-AA08-2F4EEFEEB289}"/>
+    <workbookView xWindow="4956" yWindow="840" windowWidth="18084" windowHeight="12120" xr2:uid="{529C1CFA-C348-486F-AA08-2F4EEFEEB289}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -355,7 +354,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.15840269966254217"/>
+          <c:y val="0.2384584342211461"/>
+          <c:w val="0.80454968128983895"/>
+          <c:h val="0.66792466619638646"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -971,7 +980,690 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>dry biomass (g)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:intercept val="0"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$H$2:$H$991</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="990"/>
+                <c:pt idx="0">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>18</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$I$2:$I$991</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="990"/>
+                <c:pt idx="0">
+                  <c:v>51.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>62.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>37.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>26.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>22.1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13.7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>51.3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>22.7</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>16.8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>42.8</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>25.52</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>218.88</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>24.61</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>23.37</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>18.27</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>133.22</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>61.55</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>61.83</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>52.78</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>55.01</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>133.81</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>79.069999999999993</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>154.16999999999999</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>151.26</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>73.819999999999993</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>77.97</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>50.65</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>50.5</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>48.24</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>85.11</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>99.45</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>77.08</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>41.56</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>87.79</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>62.85</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>110.47</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>61.28</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>129.38</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>156.99</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>80.510000000000005</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>153.44</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>60.01</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>100.73</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>132.59</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-19F1-4AE7-9563-2B4206BADD81}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="534074383"/>
+        <c:axId val="510178991"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="534074383"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="510178991"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="510178991"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="534074383"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1527,14 +2219,530 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>480060</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>586740</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
@@ -1567,11 +2775,47 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>251460</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50E528F6-9A9C-9776-CF84-2601BFE71994}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="MetaData"/>
@@ -2328,8 +3572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{617FA0DB-87D6-48CC-B2AB-36E698C714D8}">
   <dimension ref="A1:I991"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="I1" activeCellId="1" sqref="H1:H1048576 I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Cleaning up folders for public version
</commit_message>
<xml_diff>
--- a/rawdata/PastureMeterCalibration.xlsx
+++ b/rawdata/PastureMeterCalibration.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elwel\OneDrive\Desktop\AppraisingGrazing\rawdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC2A634D-E466-421B-B1B7-B0D11EA19BD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A6C8420-77C3-491B-A329-90135D87A37F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4956" yWindow="840" windowWidth="18084" windowHeight="12120" xr2:uid="{529C1CFA-C348-486F-AA08-2F4EEFEEB289}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{529C1CFA-C348-486F-AA08-2F4EEFEEB289}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3260,6 +3260,3766 @@
             <v>132.59</v>
           </cell>
         </row>
+        <row r="52">
+          <cell r="H52"/>
+          <cell r="I52"/>
+        </row>
+        <row r="53">
+          <cell r="H53"/>
+          <cell r="I53"/>
+        </row>
+        <row r="54">
+          <cell r="H54"/>
+          <cell r="I54"/>
+        </row>
+        <row r="55">
+          <cell r="H55"/>
+          <cell r="I55"/>
+        </row>
+        <row r="56">
+          <cell r="H56"/>
+          <cell r="I56"/>
+        </row>
+        <row r="57">
+          <cell r="H57"/>
+          <cell r="I57"/>
+        </row>
+        <row r="58">
+          <cell r="H58"/>
+          <cell r="I58"/>
+        </row>
+        <row r="59">
+          <cell r="H59"/>
+          <cell r="I59"/>
+        </row>
+        <row r="60">
+          <cell r="H60"/>
+          <cell r="I60"/>
+        </row>
+        <row r="61">
+          <cell r="H61"/>
+          <cell r="I61"/>
+        </row>
+        <row r="62">
+          <cell r="H62"/>
+          <cell r="I62"/>
+        </row>
+        <row r="63">
+          <cell r="H63"/>
+          <cell r="I63"/>
+        </row>
+        <row r="64">
+          <cell r="H64"/>
+          <cell r="I64"/>
+        </row>
+        <row r="65">
+          <cell r="H65"/>
+          <cell r="I65"/>
+        </row>
+        <row r="66">
+          <cell r="H66"/>
+          <cell r="I66"/>
+        </row>
+        <row r="67">
+          <cell r="H67"/>
+          <cell r="I67"/>
+        </row>
+        <row r="68">
+          <cell r="H68"/>
+          <cell r="I68"/>
+        </row>
+        <row r="69">
+          <cell r="H69"/>
+          <cell r="I69"/>
+        </row>
+        <row r="70">
+          <cell r="H70"/>
+          <cell r="I70"/>
+        </row>
+        <row r="71">
+          <cell r="H71"/>
+          <cell r="I71"/>
+        </row>
+        <row r="72">
+          <cell r="H72"/>
+          <cell r="I72"/>
+        </row>
+        <row r="73">
+          <cell r="H73"/>
+          <cell r="I73"/>
+        </row>
+        <row r="74">
+          <cell r="H74"/>
+          <cell r="I74"/>
+        </row>
+        <row r="75">
+          <cell r="H75"/>
+          <cell r="I75"/>
+        </row>
+        <row r="76">
+          <cell r="H76"/>
+          <cell r="I76"/>
+        </row>
+        <row r="77">
+          <cell r="H77"/>
+          <cell r="I77"/>
+        </row>
+        <row r="78">
+          <cell r="H78"/>
+          <cell r="I78"/>
+        </row>
+        <row r="79">
+          <cell r="H79"/>
+          <cell r="I79"/>
+        </row>
+        <row r="80">
+          <cell r="H80"/>
+          <cell r="I80"/>
+        </row>
+        <row r="81">
+          <cell r="H81"/>
+          <cell r="I81"/>
+        </row>
+        <row r="82">
+          <cell r="H82"/>
+          <cell r="I82"/>
+        </row>
+        <row r="83">
+          <cell r="H83"/>
+          <cell r="I83"/>
+        </row>
+        <row r="84">
+          <cell r="H84"/>
+          <cell r="I84"/>
+        </row>
+        <row r="85">
+          <cell r="H85"/>
+          <cell r="I85"/>
+        </row>
+        <row r="86">
+          <cell r="H86"/>
+          <cell r="I86"/>
+        </row>
+        <row r="87">
+          <cell r="H87"/>
+          <cell r="I87"/>
+        </row>
+        <row r="88">
+          <cell r="H88"/>
+          <cell r="I88"/>
+        </row>
+        <row r="89">
+          <cell r="H89"/>
+          <cell r="I89"/>
+        </row>
+        <row r="90">
+          <cell r="H90"/>
+          <cell r="I90"/>
+        </row>
+        <row r="91">
+          <cell r="H91"/>
+          <cell r="I91"/>
+        </row>
+        <row r="92">
+          <cell r="H92"/>
+          <cell r="I92"/>
+        </row>
+        <row r="93">
+          <cell r="H93"/>
+          <cell r="I93"/>
+        </row>
+        <row r="94">
+          <cell r="H94"/>
+          <cell r="I94"/>
+        </row>
+        <row r="95">
+          <cell r="H95"/>
+          <cell r="I95"/>
+        </row>
+        <row r="96">
+          <cell r="H96"/>
+          <cell r="I96"/>
+        </row>
+        <row r="97">
+          <cell r="H97"/>
+          <cell r="I97"/>
+        </row>
+        <row r="98">
+          <cell r="H98"/>
+          <cell r="I98"/>
+        </row>
+        <row r="99">
+          <cell r="H99"/>
+          <cell r="I99"/>
+        </row>
+        <row r="100">
+          <cell r="H100"/>
+          <cell r="I100"/>
+        </row>
+        <row r="101">
+          <cell r="H101"/>
+          <cell r="I101"/>
+        </row>
+        <row r="102">
+          <cell r="H102"/>
+          <cell r="I102"/>
+        </row>
+        <row r="103">
+          <cell r="H103"/>
+          <cell r="I103"/>
+        </row>
+        <row r="104">
+          <cell r="H104"/>
+          <cell r="I104"/>
+        </row>
+        <row r="105">
+          <cell r="H105"/>
+          <cell r="I105"/>
+        </row>
+        <row r="106">
+          <cell r="H106"/>
+          <cell r="I106"/>
+        </row>
+        <row r="107">
+          <cell r="H107"/>
+          <cell r="I107"/>
+        </row>
+        <row r="108">
+          <cell r="H108"/>
+          <cell r="I108"/>
+        </row>
+        <row r="109">
+          <cell r="H109"/>
+          <cell r="I109"/>
+        </row>
+        <row r="110">
+          <cell r="H110"/>
+          <cell r="I110"/>
+        </row>
+        <row r="111">
+          <cell r="H111"/>
+          <cell r="I111"/>
+        </row>
+        <row r="112">
+          <cell r="H112"/>
+          <cell r="I112"/>
+        </row>
+        <row r="113">
+          <cell r="H113"/>
+          <cell r="I113"/>
+        </row>
+        <row r="114">
+          <cell r="H114"/>
+          <cell r="I114"/>
+        </row>
+        <row r="115">
+          <cell r="H115"/>
+          <cell r="I115"/>
+        </row>
+        <row r="116">
+          <cell r="H116"/>
+          <cell r="I116"/>
+        </row>
+        <row r="117">
+          <cell r="H117"/>
+          <cell r="I117"/>
+        </row>
+        <row r="118">
+          <cell r="H118"/>
+          <cell r="I118"/>
+        </row>
+        <row r="119">
+          <cell r="H119"/>
+          <cell r="I119"/>
+        </row>
+        <row r="120">
+          <cell r="H120"/>
+          <cell r="I120"/>
+        </row>
+        <row r="121">
+          <cell r="H121"/>
+          <cell r="I121"/>
+        </row>
+        <row r="122">
+          <cell r="H122"/>
+          <cell r="I122"/>
+        </row>
+        <row r="123">
+          <cell r="H123"/>
+          <cell r="I123"/>
+        </row>
+        <row r="124">
+          <cell r="H124"/>
+          <cell r="I124"/>
+        </row>
+        <row r="125">
+          <cell r="H125"/>
+          <cell r="I125"/>
+        </row>
+        <row r="126">
+          <cell r="H126"/>
+          <cell r="I126"/>
+        </row>
+        <row r="127">
+          <cell r="H127"/>
+          <cell r="I127"/>
+        </row>
+        <row r="128">
+          <cell r="H128"/>
+          <cell r="I128"/>
+        </row>
+        <row r="129">
+          <cell r="H129"/>
+          <cell r="I129"/>
+        </row>
+        <row r="130">
+          <cell r="H130"/>
+          <cell r="I130"/>
+        </row>
+        <row r="131">
+          <cell r="H131"/>
+          <cell r="I131"/>
+        </row>
+        <row r="132">
+          <cell r="H132"/>
+          <cell r="I132"/>
+        </row>
+        <row r="133">
+          <cell r="H133"/>
+          <cell r="I133"/>
+        </row>
+        <row r="134">
+          <cell r="H134"/>
+          <cell r="I134"/>
+        </row>
+        <row r="135">
+          <cell r="H135"/>
+          <cell r="I135"/>
+        </row>
+        <row r="136">
+          <cell r="H136"/>
+          <cell r="I136"/>
+        </row>
+        <row r="137">
+          <cell r="H137"/>
+          <cell r="I137"/>
+        </row>
+        <row r="138">
+          <cell r="H138"/>
+          <cell r="I138"/>
+        </row>
+        <row r="139">
+          <cell r="H139"/>
+          <cell r="I139"/>
+        </row>
+        <row r="140">
+          <cell r="H140"/>
+          <cell r="I140"/>
+        </row>
+        <row r="141">
+          <cell r="H141"/>
+          <cell r="I141"/>
+        </row>
+        <row r="142">
+          <cell r="H142"/>
+          <cell r="I142"/>
+        </row>
+        <row r="143">
+          <cell r="H143"/>
+          <cell r="I143"/>
+        </row>
+        <row r="144">
+          <cell r="H144"/>
+          <cell r="I144"/>
+        </row>
+        <row r="145">
+          <cell r="H145"/>
+          <cell r="I145"/>
+        </row>
+        <row r="146">
+          <cell r="H146"/>
+          <cell r="I146"/>
+        </row>
+        <row r="147">
+          <cell r="H147"/>
+          <cell r="I147"/>
+        </row>
+        <row r="148">
+          <cell r="H148"/>
+          <cell r="I148"/>
+        </row>
+        <row r="149">
+          <cell r="H149"/>
+          <cell r="I149"/>
+        </row>
+        <row r="150">
+          <cell r="H150"/>
+          <cell r="I150"/>
+        </row>
+        <row r="151">
+          <cell r="H151"/>
+          <cell r="I151"/>
+        </row>
+        <row r="152">
+          <cell r="H152"/>
+          <cell r="I152"/>
+        </row>
+        <row r="153">
+          <cell r="H153"/>
+          <cell r="I153"/>
+        </row>
+        <row r="154">
+          <cell r="H154"/>
+          <cell r="I154"/>
+        </row>
+        <row r="155">
+          <cell r="H155"/>
+          <cell r="I155"/>
+        </row>
+        <row r="156">
+          <cell r="H156"/>
+          <cell r="I156"/>
+        </row>
+        <row r="157">
+          <cell r="H157"/>
+          <cell r="I157"/>
+        </row>
+        <row r="158">
+          <cell r="H158"/>
+          <cell r="I158"/>
+        </row>
+        <row r="159">
+          <cell r="H159"/>
+          <cell r="I159"/>
+        </row>
+        <row r="160">
+          <cell r="H160"/>
+          <cell r="I160"/>
+        </row>
+        <row r="161">
+          <cell r="H161"/>
+          <cell r="I161"/>
+        </row>
+        <row r="162">
+          <cell r="H162"/>
+          <cell r="I162"/>
+        </row>
+        <row r="163">
+          <cell r="H163"/>
+          <cell r="I163"/>
+        </row>
+        <row r="164">
+          <cell r="H164"/>
+          <cell r="I164"/>
+        </row>
+        <row r="165">
+          <cell r="H165"/>
+          <cell r="I165"/>
+        </row>
+        <row r="166">
+          <cell r="H166"/>
+          <cell r="I166"/>
+        </row>
+        <row r="167">
+          <cell r="H167"/>
+          <cell r="I167"/>
+        </row>
+        <row r="168">
+          <cell r="H168"/>
+          <cell r="I168"/>
+        </row>
+        <row r="169">
+          <cell r="H169"/>
+          <cell r="I169"/>
+        </row>
+        <row r="170">
+          <cell r="H170"/>
+          <cell r="I170"/>
+        </row>
+        <row r="171">
+          <cell r="H171"/>
+          <cell r="I171"/>
+        </row>
+        <row r="172">
+          <cell r="H172"/>
+          <cell r="I172"/>
+        </row>
+        <row r="173">
+          <cell r="H173"/>
+          <cell r="I173"/>
+        </row>
+        <row r="174">
+          <cell r="H174"/>
+          <cell r="I174"/>
+        </row>
+        <row r="175">
+          <cell r="H175"/>
+          <cell r="I175"/>
+        </row>
+        <row r="176">
+          <cell r="H176"/>
+          <cell r="I176"/>
+        </row>
+        <row r="177">
+          <cell r="H177"/>
+          <cell r="I177"/>
+        </row>
+        <row r="178">
+          <cell r="H178"/>
+          <cell r="I178"/>
+        </row>
+        <row r="179">
+          <cell r="H179"/>
+          <cell r="I179"/>
+        </row>
+        <row r="180">
+          <cell r="H180"/>
+          <cell r="I180"/>
+        </row>
+        <row r="181">
+          <cell r="H181"/>
+          <cell r="I181"/>
+        </row>
+        <row r="182">
+          <cell r="H182"/>
+          <cell r="I182"/>
+        </row>
+        <row r="183">
+          <cell r="H183"/>
+          <cell r="I183"/>
+        </row>
+        <row r="184">
+          <cell r="H184"/>
+          <cell r="I184"/>
+        </row>
+        <row r="185">
+          <cell r="H185"/>
+          <cell r="I185"/>
+        </row>
+        <row r="186">
+          <cell r="H186"/>
+          <cell r="I186"/>
+        </row>
+        <row r="187">
+          <cell r="H187"/>
+          <cell r="I187"/>
+        </row>
+        <row r="188">
+          <cell r="H188"/>
+          <cell r="I188"/>
+        </row>
+        <row r="189">
+          <cell r="H189"/>
+          <cell r="I189"/>
+        </row>
+        <row r="190">
+          <cell r="H190"/>
+          <cell r="I190"/>
+        </row>
+        <row r="191">
+          <cell r="H191"/>
+          <cell r="I191"/>
+        </row>
+        <row r="192">
+          <cell r="H192"/>
+          <cell r="I192"/>
+        </row>
+        <row r="193">
+          <cell r="H193"/>
+          <cell r="I193"/>
+        </row>
+        <row r="194">
+          <cell r="H194"/>
+          <cell r="I194"/>
+        </row>
+        <row r="195">
+          <cell r="H195"/>
+          <cell r="I195"/>
+        </row>
+        <row r="196">
+          <cell r="H196"/>
+          <cell r="I196"/>
+        </row>
+        <row r="197">
+          <cell r="H197"/>
+          <cell r="I197"/>
+        </row>
+        <row r="198">
+          <cell r="H198"/>
+          <cell r="I198"/>
+        </row>
+        <row r="199">
+          <cell r="H199"/>
+          <cell r="I199"/>
+        </row>
+        <row r="200">
+          <cell r="H200"/>
+          <cell r="I200"/>
+        </row>
+        <row r="201">
+          <cell r="H201"/>
+          <cell r="I201"/>
+        </row>
+        <row r="202">
+          <cell r="H202"/>
+          <cell r="I202"/>
+        </row>
+        <row r="203">
+          <cell r="H203"/>
+          <cell r="I203"/>
+        </row>
+        <row r="204">
+          <cell r="H204"/>
+          <cell r="I204"/>
+        </row>
+        <row r="205">
+          <cell r="H205"/>
+          <cell r="I205"/>
+        </row>
+        <row r="206">
+          <cell r="H206"/>
+          <cell r="I206"/>
+        </row>
+        <row r="207">
+          <cell r="H207"/>
+          <cell r="I207"/>
+        </row>
+        <row r="208">
+          <cell r="H208"/>
+          <cell r="I208"/>
+        </row>
+        <row r="209">
+          <cell r="H209"/>
+          <cell r="I209"/>
+        </row>
+        <row r="210">
+          <cell r="H210"/>
+          <cell r="I210"/>
+        </row>
+        <row r="211">
+          <cell r="H211"/>
+          <cell r="I211"/>
+        </row>
+        <row r="212">
+          <cell r="H212"/>
+          <cell r="I212"/>
+        </row>
+        <row r="213">
+          <cell r="H213"/>
+          <cell r="I213"/>
+        </row>
+        <row r="214">
+          <cell r="H214"/>
+          <cell r="I214"/>
+        </row>
+        <row r="215">
+          <cell r="H215"/>
+          <cell r="I215"/>
+        </row>
+        <row r="216">
+          <cell r="H216"/>
+          <cell r="I216"/>
+        </row>
+        <row r="217">
+          <cell r="H217"/>
+          <cell r="I217"/>
+        </row>
+        <row r="218">
+          <cell r="H218"/>
+          <cell r="I218"/>
+        </row>
+        <row r="219">
+          <cell r="H219"/>
+          <cell r="I219"/>
+        </row>
+        <row r="220">
+          <cell r="H220"/>
+          <cell r="I220"/>
+        </row>
+        <row r="221">
+          <cell r="H221"/>
+          <cell r="I221"/>
+        </row>
+        <row r="222">
+          <cell r="H222"/>
+          <cell r="I222"/>
+        </row>
+        <row r="223">
+          <cell r="H223"/>
+          <cell r="I223"/>
+        </row>
+        <row r="224">
+          <cell r="H224"/>
+          <cell r="I224"/>
+        </row>
+        <row r="225">
+          <cell r="H225"/>
+          <cell r="I225"/>
+        </row>
+        <row r="226">
+          <cell r="H226"/>
+          <cell r="I226"/>
+        </row>
+        <row r="227">
+          <cell r="H227"/>
+          <cell r="I227"/>
+        </row>
+        <row r="228">
+          <cell r="H228"/>
+          <cell r="I228"/>
+        </row>
+        <row r="229">
+          <cell r="H229"/>
+          <cell r="I229"/>
+        </row>
+        <row r="230">
+          <cell r="H230"/>
+          <cell r="I230"/>
+        </row>
+        <row r="231">
+          <cell r="H231"/>
+          <cell r="I231"/>
+        </row>
+        <row r="232">
+          <cell r="H232"/>
+          <cell r="I232"/>
+        </row>
+        <row r="233">
+          <cell r="H233"/>
+          <cell r="I233"/>
+        </row>
+        <row r="234">
+          <cell r="H234"/>
+          <cell r="I234"/>
+        </row>
+        <row r="235">
+          <cell r="H235"/>
+          <cell r="I235"/>
+        </row>
+        <row r="236">
+          <cell r="H236"/>
+          <cell r="I236"/>
+        </row>
+        <row r="237">
+          <cell r="H237"/>
+          <cell r="I237"/>
+        </row>
+        <row r="238">
+          <cell r="H238"/>
+          <cell r="I238"/>
+        </row>
+        <row r="239">
+          <cell r="H239"/>
+          <cell r="I239"/>
+        </row>
+        <row r="240">
+          <cell r="H240"/>
+          <cell r="I240"/>
+        </row>
+        <row r="241">
+          <cell r="H241"/>
+          <cell r="I241"/>
+        </row>
+        <row r="242">
+          <cell r="H242"/>
+          <cell r="I242"/>
+        </row>
+        <row r="243">
+          <cell r="H243"/>
+          <cell r="I243"/>
+        </row>
+        <row r="244">
+          <cell r="H244"/>
+          <cell r="I244"/>
+        </row>
+        <row r="245">
+          <cell r="H245"/>
+          <cell r="I245"/>
+        </row>
+        <row r="246">
+          <cell r="H246"/>
+          <cell r="I246"/>
+        </row>
+        <row r="247">
+          <cell r="H247"/>
+          <cell r="I247"/>
+        </row>
+        <row r="248">
+          <cell r="H248"/>
+          <cell r="I248"/>
+        </row>
+        <row r="249">
+          <cell r="H249"/>
+          <cell r="I249"/>
+        </row>
+        <row r="250">
+          <cell r="H250"/>
+          <cell r="I250"/>
+        </row>
+        <row r="251">
+          <cell r="H251"/>
+          <cell r="I251"/>
+        </row>
+        <row r="252">
+          <cell r="H252"/>
+          <cell r="I252"/>
+        </row>
+        <row r="253">
+          <cell r="H253"/>
+          <cell r="I253"/>
+        </row>
+        <row r="254">
+          <cell r="H254"/>
+          <cell r="I254"/>
+        </row>
+        <row r="255">
+          <cell r="H255"/>
+          <cell r="I255"/>
+        </row>
+        <row r="256">
+          <cell r="H256"/>
+          <cell r="I256"/>
+        </row>
+        <row r="257">
+          <cell r="H257"/>
+          <cell r="I257"/>
+        </row>
+        <row r="258">
+          <cell r="H258"/>
+          <cell r="I258"/>
+        </row>
+        <row r="259">
+          <cell r="H259"/>
+          <cell r="I259"/>
+        </row>
+        <row r="260">
+          <cell r="H260"/>
+          <cell r="I260"/>
+        </row>
+        <row r="261">
+          <cell r="H261"/>
+          <cell r="I261"/>
+        </row>
+        <row r="262">
+          <cell r="H262"/>
+          <cell r="I262"/>
+        </row>
+        <row r="263">
+          <cell r="H263"/>
+          <cell r="I263"/>
+        </row>
+        <row r="264">
+          <cell r="H264"/>
+          <cell r="I264"/>
+        </row>
+        <row r="265">
+          <cell r="H265"/>
+          <cell r="I265"/>
+        </row>
+        <row r="266">
+          <cell r="H266"/>
+          <cell r="I266"/>
+        </row>
+        <row r="267">
+          <cell r="H267"/>
+          <cell r="I267"/>
+        </row>
+        <row r="268">
+          <cell r="H268"/>
+          <cell r="I268"/>
+        </row>
+        <row r="269">
+          <cell r="H269"/>
+          <cell r="I269"/>
+        </row>
+        <row r="270">
+          <cell r="H270"/>
+          <cell r="I270"/>
+        </row>
+        <row r="271">
+          <cell r="H271"/>
+          <cell r="I271"/>
+        </row>
+        <row r="272">
+          <cell r="H272"/>
+          <cell r="I272"/>
+        </row>
+        <row r="273">
+          <cell r="H273"/>
+          <cell r="I273"/>
+        </row>
+        <row r="274">
+          <cell r="H274"/>
+          <cell r="I274"/>
+        </row>
+        <row r="275">
+          <cell r="H275"/>
+          <cell r="I275"/>
+        </row>
+        <row r="276">
+          <cell r="H276"/>
+          <cell r="I276"/>
+        </row>
+        <row r="277">
+          <cell r="H277"/>
+          <cell r="I277"/>
+        </row>
+        <row r="278">
+          <cell r="H278"/>
+          <cell r="I278"/>
+        </row>
+        <row r="279">
+          <cell r="H279"/>
+          <cell r="I279"/>
+        </row>
+        <row r="280">
+          <cell r="H280"/>
+          <cell r="I280"/>
+        </row>
+        <row r="281">
+          <cell r="H281"/>
+          <cell r="I281"/>
+        </row>
+        <row r="282">
+          <cell r="H282"/>
+          <cell r="I282"/>
+        </row>
+        <row r="283">
+          <cell r="H283"/>
+          <cell r="I283"/>
+        </row>
+        <row r="284">
+          <cell r="H284"/>
+          <cell r="I284"/>
+        </row>
+        <row r="285">
+          <cell r="H285"/>
+          <cell r="I285"/>
+        </row>
+        <row r="286">
+          <cell r="H286"/>
+          <cell r="I286"/>
+        </row>
+        <row r="287">
+          <cell r="H287"/>
+          <cell r="I287"/>
+        </row>
+        <row r="288">
+          <cell r="H288"/>
+          <cell r="I288"/>
+        </row>
+        <row r="289">
+          <cell r="H289"/>
+          <cell r="I289"/>
+        </row>
+        <row r="290">
+          <cell r="H290"/>
+          <cell r="I290"/>
+        </row>
+        <row r="291">
+          <cell r="H291"/>
+          <cell r="I291"/>
+        </row>
+        <row r="292">
+          <cell r="H292"/>
+          <cell r="I292"/>
+        </row>
+        <row r="293">
+          <cell r="H293"/>
+          <cell r="I293"/>
+        </row>
+        <row r="294">
+          <cell r="H294"/>
+          <cell r="I294"/>
+        </row>
+        <row r="295">
+          <cell r="H295"/>
+          <cell r="I295"/>
+        </row>
+        <row r="296">
+          <cell r="H296"/>
+          <cell r="I296"/>
+        </row>
+        <row r="297">
+          <cell r="H297"/>
+          <cell r="I297"/>
+        </row>
+        <row r="298">
+          <cell r="H298"/>
+          <cell r="I298"/>
+        </row>
+        <row r="299">
+          <cell r="H299"/>
+          <cell r="I299"/>
+        </row>
+        <row r="300">
+          <cell r="H300"/>
+          <cell r="I300"/>
+        </row>
+        <row r="301">
+          <cell r="H301"/>
+          <cell r="I301"/>
+        </row>
+        <row r="302">
+          <cell r="H302"/>
+          <cell r="I302"/>
+        </row>
+        <row r="303">
+          <cell r="H303"/>
+          <cell r="I303"/>
+        </row>
+        <row r="304">
+          <cell r="H304"/>
+          <cell r="I304"/>
+        </row>
+        <row r="305">
+          <cell r="H305"/>
+          <cell r="I305"/>
+        </row>
+        <row r="306">
+          <cell r="H306"/>
+          <cell r="I306"/>
+        </row>
+        <row r="307">
+          <cell r="H307"/>
+          <cell r="I307"/>
+        </row>
+        <row r="308">
+          <cell r="H308"/>
+          <cell r="I308"/>
+        </row>
+        <row r="309">
+          <cell r="H309"/>
+          <cell r="I309"/>
+        </row>
+        <row r="310">
+          <cell r="H310"/>
+          <cell r="I310"/>
+        </row>
+        <row r="311">
+          <cell r="H311"/>
+          <cell r="I311"/>
+        </row>
+        <row r="312">
+          <cell r="H312"/>
+          <cell r="I312"/>
+        </row>
+        <row r="313">
+          <cell r="H313"/>
+          <cell r="I313"/>
+        </row>
+        <row r="314">
+          <cell r="H314"/>
+          <cell r="I314"/>
+        </row>
+        <row r="315">
+          <cell r="H315"/>
+          <cell r="I315"/>
+        </row>
+        <row r="316">
+          <cell r="H316"/>
+          <cell r="I316"/>
+        </row>
+        <row r="317">
+          <cell r="H317"/>
+          <cell r="I317"/>
+        </row>
+        <row r="318">
+          <cell r="H318"/>
+          <cell r="I318"/>
+        </row>
+        <row r="319">
+          <cell r="H319"/>
+          <cell r="I319"/>
+        </row>
+        <row r="320">
+          <cell r="H320"/>
+          <cell r="I320"/>
+        </row>
+        <row r="321">
+          <cell r="H321"/>
+          <cell r="I321"/>
+        </row>
+        <row r="322">
+          <cell r="H322"/>
+          <cell r="I322"/>
+        </row>
+        <row r="323">
+          <cell r="H323"/>
+          <cell r="I323"/>
+        </row>
+        <row r="324">
+          <cell r="H324"/>
+          <cell r="I324"/>
+        </row>
+        <row r="325">
+          <cell r="H325"/>
+          <cell r="I325"/>
+        </row>
+        <row r="326">
+          <cell r="H326"/>
+          <cell r="I326"/>
+        </row>
+        <row r="327">
+          <cell r="H327"/>
+          <cell r="I327"/>
+        </row>
+        <row r="328">
+          <cell r="H328"/>
+          <cell r="I328"/>
+        </row>
+        <row r="329">
+          <cell r="H329"/>
+          <cell r="I329"/>
+        </row>
+        <row r="330">
+          <cell r="H330"/>
+          <cell r="I330"/>
+        </row>
+        <row r="331">
+          <cell r="H331"/>
+          <cell r="I331"/>
+        </row>
+        <row r="332">
+          <cell r="H332"/>
+          <cell r="I332"/>
+        </row>
+        <row r="333">
+          <cell r="H333"/>
+          <cell r="I333"/>
+        </row>
+        <row r="334">
+          <cell r="H334"/>
+          <cell r="I334"/>
+        </row>
+        <row r="335">
+          <cell r="H335"/>
+          <cell r="I335"/>
+        </row>
+        <row r="336">
+          <cell r="H336"/>
+          <cell r="I336"/>
+        </row>
+        <row r="337">
+          <cell r="H337"/>
+          <cell r="I337"/>
+        </row>
+        <row r="338">
+          <cell r="H338"/>
+          <cell r="I338"/>
+        </row>
+        <row r="339">
+          <cell r="H339"/>
+          <cell r="I339"/>
+        </row>
+        <row r="340">
+          <cell r="H340"/>
+          <cell r="I340"/>
+        </row>
+        <row r="341">
+          <cell r="H341"/>
+          <cell r="I341"/>
+        </row>
+        <row r="342">
+          <cell r="H342"/>
+          <cell r="I342"/>
+        </row>
+        <row r="343">
+          <cell r="H343"/>
+          <cell r="I343"/>
+        </row>
+        <row r="344">
+          <cell r="H344"/>
+          <cell r="I344"/>
+        </row>
+        <row r="345">
+          <cell r="H345"/>
+          <cell r="I345"/>
+        </row>
+        <row r="346">
+          <cell r="H346"/>
+          <cell r="I346"/>
+        </row>
+        <row r="347">
+          <cell r="H347"/>
+          <cell r="I347"/>
+        </row>
+        <row r="348">
+          <cell r="H348"/>
+          <cell r="I348"/>
+        </row>
+        <row r="349">
+          <cell r="H349"/>
+          <cell r="I349"/>
+        </row>
+        <row r="350">
+          <cell r="H350"/>
+          <cell r="I350"/>
+        </row>
+        <row r="351">
+          <cell r="H351"/>
+          <cell r="I351"/>
+        </row>
+        <row r="352">
+          <cell r="H352"/>
+          <cell r="I352"/>
+        </row>
+        <row r="353">
+          <cell r="H353"/>
+          <cell r="I353"/>
+        </row>
+        <row r="354">
+          <cell r="H354"/>
+          <cell r="I354"/>
+        </row>
+        <row r="355">
+          <cell r="H355"/>
+          <cell r="I355"/>
+        </row>
+        <row r="356">
+          <cell r="H356"/>
+          <cell r="I356"/>
+        </row>
+        <row r="357">
+          <cell r="H357"/>
+          <cell r="I357"/>
+        </row>
+        <row r="358">
+          <cell r="H358"/>
+          <cell r="I358"/>
+        </row>
+        <row r="359">
+          <cell r="H359"/>
+          <cell r="I359"/>
+        </row>
+        <row r="360">
+          <cell r="H360"/>
+          <cell r="I360"/>
+        </row>
+        <row r="361">
+          <cell r="H361"/>
+          <cell r="I361"/>
+        </row>
+        <row r="362">
+          <cell r="H362"/>
+          <cell r="I362"/>
+        </row>
+        <row r="363">
+          <cell r="H363"/>
+          <cell r="I363"/>
+        </row>
+        <row r="364">
+          <cell r="H364"/>
+          <cell r="I364"/>
+        </row>
+        <row r="365">
+          <cell r="H365"/>
+          <cell r="I365"/>
+        </row>
+        <row r="366">
+          <cell r="H366"/>
+          <cell r="I366"/>
+        </row>
+        <row r="367">
+          <cell r="H367"/>
+          <cell r="I367"/>
+        </row>
+        <row r="368">
+          <cell r="H368"/>
+          <cell r="I368"/>
+        </row>
+        <row r="369">
+          <cell r="H369"/>
+          <cell r="I369"/>
+        </row>
+        <row r="370">
+          <cell r="H370"/>
+          <cell r="I370"/>
+        </row>
+        <row r="371">
+          <cell r="H371"/>
+          <cell r="I371"/>
+        </row>
+        <row r="372">
+          <cell r="H372"/>
+          <cell r="I372"/>
+        </row>
+        <row r="373">
+          <cell r="H373"/>
+          <cell r="I373"/>
+        </row>
+        <row r="374">
+          <cell r="H374"/>
+          <cell r="I374"/>
+        </row>
+        <row r="375">
+          <cell r="H375"/>
+          <cell r="I375"/>
+        </row>
+        <row r="376">
+          <cell r="H376"/>
+          <cell r="I376"/>
+        </row>
+        <row r="377">
+          <cell r="H377"/>
+          <cell r="I377"/>
+        </row>
+        <row r="378">
+          <cell r="H378"/>
+          <cell r="I378"/>
+        </row>
+        <row r="379">
+          <cell r="H379"/>
+          <cell r="I379"/>
+        </row>
+        <row r="380">
+          <cell r="H380"/>
+          <cell r="I380"/>
+        </row>
+        <row r="381">
+          <cell r="H381"/>
+          <cell r="I381"/>
+        </row>
+        <row r="382">
+          <cell r="H382"/>
+          <cell r="I382"/>
+        </row>
+        <row r="383">
+          <cell r="H383"/>
+          <cell r="I383"/>
+        </row>
+        <row r="384">
+          <cell r="H384"/>
+          <cell r="I384"/>
+        </row>
+        <row r="385">
+          <cell r="H385"/>
+          <cell r="I385"/>
+        </row>
+        <row r="386">
+          <cell r="H386"/>
+          <cell r="I386"/>
+        </row>
+        <row r="387">
+          <cell r="H387"/>
+          <cell r="I387"/>
+        </row>
+        <row r="388">
+          <cell r="H388"/>
+          <cell r="I388"/>
+        </row>
+        <row r="389">
+          <cell r="H389"/>
+          <cell r="I389"/>
+        </row>
+        <row r="390">
+          <cell r="H390"/>
+          <cell r="I390"/>
+        </row>
+        <row r="391">
+          <cell r="H391"/>
+          <cell r="I391"/>
+        </row>
+        <row r="392">
+          <cell r="H392"/>
+          <cell r="I392"/>
+        </row>
+        <row r="393">
+          <cell r="H393"/>
+          <cell r="I393"/>
+        </row>
+        <row r="394">
+          <cell r="H394"/>
+          <cell r="I394"/>
+        </row>
+        <row r="395">
+          <cell r="H395"/>
+          <cell r="I395"/>
+        </row>
+        <row r="396">
+          <cell r="H396"/>
+          <cell r="I396"/>
+        </row>
+        <row r="397">
+          <cell r="H397"/>
+          <cell r="I397"/>
+        </row>
+        <row r="398">
+          <cell r="H398"/>
+          <cell r="I398"/>
+        </row>
+        <row r="399">
+          <cell r="H399"/>
+          <cell r="I399"/>
+        </row>
+        <row r="400">
+          <cell r="H400"/>
+          <cell r="I400"/>
+        </row>
+        <row r="401">
+          <cell r="H401"/>
+          <cell r="I401"/>
+        </row>
+        <row r="402">
+          <cell r="H402"/>
+          <cell r="I402"/>
+        </row>
+        <row r="403">
+          <cell r="H403"/>
+          <cell r="I403"/>
+        </row>
+        <row r="404">
+          <cell r="H404"/>
+          <cell r="I404"/>
+        </row>
+        <row r="405">
+          <cell r="H405"/>
+          <cell r="I405"/>
+        </row>
+        <row r="406">
+          <cell r="H406"/>
+          <cell r="I406"/>
+        </row>
+        <row r="407">
+          <cell r="H407"/>
+          <cell r="I407"/>
+        </row>
+        <row r="408">
+          <cell r="H408"/>
+          <cell r="I408"/>
+        </row>
+        <row r="409">
+          <cell r="H409"/>
+          <cell r="I409"/>
+        </row>
+        <row r="410">
+          <cell r="H410"/>
+          <cell r="I410"/>
+        </row>
+        <row r="411">
+          <cell r="H411"/>
+          <cell r="I411"/>
+        </row>
+        <row r="412">
+          <cell r="H412"/>
+          <cell r="I412"/>
+        </row>
+        <row r="413">
+          <cell r="H413"/>
+          <cell r="I413"/>
+        </row>
+        <row r="414">
+          <cell r="H414"/>
+          <cell r="I414"/>
+        </row>
+        <row r="415">
+          <cell r="H415"/>
+          <cell r="I415"/>
+        </row>
+        <row r="416">
+          <cell r="H416"/>
+          <cell r="I416"/>
+        </row>
+        <row r="417">
+          <cell r="H417"/>
+          <cell r="I417"/>
+        </row>
+        <row r="418">
+          <cell r="H418"/>
+          <cell r="I418"/>
+        </row>
+        <row r="419">
+          <cell r="H419"/>
+          <cell r="I419"/>
+        </row>
+        <row r="420">
+          <cell r="H420"/>
+          <cell r="I420"/>
+        </row>
+        <row r="421">
+          <cell r="H421"/>
+          <cell r="I421"/>
+        </row>
+        <row r="422">
+          <cell r="H422"/>
+          <cell r="I422"/>
+        </row>
+        <row r="423">
+          <cell r="H423"/>
+          <cell r="I423"/>
+        </row>
+        <row r="424">
+          <cell r="H424"/>
+          <cell r="I424"/>
+        </row>
+        <row r="425">
+          <cell r="H425"/>
+          <cell r="I425"/>
+        </row>
+        <row r="426">
+          <cell r="H426"/>
+          <cell r="I426"/>
+        </row>
+        <row r="427">
+          <cell r="H427"/>
+          <cell r="I427"/>
+        </row>
+        <row r="428">
+          <cell r="H428"/>
+          <cell r="I428"/>
+        </row>
+        <row r="429">
+          <cell r="H429"/>
+          <cell r="I429"/>
+        </row>
+        <row r="430">
+          <cell r="H430"/>
+          <cell r="I430"/>
+        </row>
+        <row r="431">
+          <cell r="H431"/>
+          <cell r="I431"/>
+        </row>
+        <row r="432">
+          <cell r="H432"/>
+          <cell r="I432"/>
+        </row>
+        <row r="433">
+          <cell r="H433"/>
+          <cell r="I433"/>
+        </row>
+        <row r="434">
+          <cell r="H434"/>
+          <cell r="I434"/>
+        </row>
+        <row r="435">
+          <cell r="H435"/>
+          <cell r="I435"/>
+        </row>
+        <row r="436">
+          <cell r="H436"/>
+          <cell r="I436"/>
+        </row>
+        <row r="437">
+          <cell r="H437"/>
+          <cell r="I437"/>
+        </row>
+        <row r="438">
+          <cell r="H438"/>
+          <cell r="I438"/>
+        </row>
+        <row r="439">
+          <cell r="H439"/>
+          <cell r="I439"/>
+        </row>
+        <row r="440">
+          <cell r="H440"/>
+          <cell r="I440"/>
+        </row>
+        <row r="441">
+          <cell r="H441"/>
+          <cell r="I441"/>
+        </row>
+        <row r="442">
+          <cell r="H442"/>
+          <cell r="I442"/>
+        </row>
+        <row r="443">
+          <cell r="H443"/>
+          <cell r="I443"/>
+        </row>
+        <row r="444">
+          <cell r="H444"/>
+          <cell r="I444"/>
+        </row>
+        <row r="445">
+          <cell r="H445"/>
+          <cell r="I445"/>
+        </row>
+        <row r="446">
+          <cell r="H446"/>
+          <cell r="I446"/>
+        </row>
+        <row r="447">
+          <cell r="H447"/>
+          <cell r="I447"/>
+        </row>
+        <row r="448">
+          <cell r="H448"/>
+          <cell r="I448"/>
+        </row>
+        <row r="449">
+          <cell r="H449"/>
+          <cell r="I449"/>
+        </row>
+        <row r="450">
+          <cell r="H450"/>
+          <cell r="I450"/>
+        </row>
+        <row r="451">
+          <cell r="H451"/>
+          <cell r="I451"/>
+        </row>
+        <row r="452">
+          <cell r="H452"/>
+          <cell r="I452"/>
+        </row>
+        <row r="453">
+          <cell r="H453"/>
+          <cell r="I453"/>
+        </row>
+        <row r="454">
+          <cell r="H454"/>
+          <cell r="I454"/>
+        </row>
+        <row r="455">
+          <cell r="H455"/>
+          <cell r="I455"/>
+        </row>
+        <row r="456">
+          <cell r="H456"/>
+          <cell r="I456"/>
+        </row>
+        <row r="457">
+          <cell r="H457"/>
+          <cell r="I457"/>
+        </row>
+        <row r="458">
+          <cell r="H458"/>
+          <cell r="I458"/>
+        </row>
+        <row r="459">
+          <cell r="H459"/>
+          <cell r="I459"/>
+        </row>
+        <row r="460">
+          <cell r="H460"/>
+          <cell r="I460"/>
+        </row>
+        <row r="461">
+          <cell r="H461"/>
+          <cell r="I461"/>
+        </row>
+        <row r="462">
+          <cell r="H462"/>
+          <cell r="I462"/>
+        </row>
+        <row r="463">
+          <cell r="H463"/>
+          <cell r="I463"/>
+        </row>
+        <row r="464">
+          <cell r="H464"/>
+          <cell r="I464"/>
+        </row>
+        <row r="465">
+          <cell r="H465"/>
+          <cell r="I465"/>
+        </row>
+        <row r="466">
+          <cell r="H466"/>
+          <cell r="I466"/>
+        </row>
+        <row r="467">
+          <cell r="H467"/>
+          <cell r="I467"/>
+        </row>
+        <row r="468">
+          <cell r="H468"/>
+          <cell r="I468"/>
+        </row>
+        <row r="469">
+          <cell r="H469"/>
+          <cell r="I469"/>
+        </row>
+        <row r="470">
+          <cell r="H470"/>
+          <cell r="I470"/>
+        </row>
+        <row r="471">
+          <cell r="H471"/>
+          <cell r="I471"/>
+        </row>
+        <row r="472">
+          <cell r="H472"/>
+          <cell r="I472"/>
+        </row>
+        <row r="473">
+          <cell r="H473"/>
+          <cell r="I473"/>
+        </row>
+        <row r="474">
+          <cell r="H474"/>
+          <cell r="I474"/>
+        </row>
+        <row r="475">
+          <cell r="H475"/>
+          <cell r="I475"/>
+        </row>
+        <row r="476">
+          <cell r="H476"/>
+          <cell r="I476"/>
+        </row>
+        <row r="477">
+          <cell r="H477"/>
+          <cell r="I477"/>
+        </row>
+        <row r="478">
+          <cell r="H478"/>
+          <cell r="I478"/>
+        </row>
+        <row r="479">
+          <cell r="H479"/>
+          <cell r="I479"/>
+        </row>
+        <row r="480">
+          <cell r="H480"/>
+          <cell r="I480"/>
+        </row>
+        <row r="481">
+          <cell r="H481"/>
+          <cell r="I481"/>
+        </row>
+        <row r="482">
+          <cell r="H482"/>
+          <cell r="I482"/>
+        </row>
+        <row r="483">
+          <cell r="H483"/>
+          <cell r="I483"/>
+        </row>
+        <row r="484">
+          <cell r="H484"/>
+          <cell r="I484"/>
+        </row>
+        <row r="485">
+          <cell r="H485"/>
+          <cell r="I485"/>
+        </row>
+        <row r="486">
+          <cell r="H486"/>
+          <cell r="I486"/>
+        </row>
+        <row r="487">
+          <cell r="H487"/>
+          <cell r="I487"/>
+        </row>
+        <row r="488">
+          <cell r="H488"/>
+          <cell r="I488"/>
+        </row>
+        <row r="489">
+          <cell r="H489"/>
+          <cell r="I489"/>
+        </row>
+        <row r="490">
+          <cell r="H490"/>
+          <cell r="I490"/>
+        </row>
+        <row r="491">
+          <cell r="H491"/>
+          <cell r="I491"/>
+        </row>
+        <row r="492">
+          <cell r="H492"/>
+          <cell r="I492"/>
+        </row>
+        <row r="493">
+          <cell r="H493"/>
+          <cell r="I493"/>
+        </row>
+        <row r="494">
+          <cell r="H494"/>
+          <cell r="I494"/>
+        </row>
+        <row r="495">
+          <cell r="H495"/>
+          <cell r="I495"/>
+        </row>
+        <row r="496">
+          <cell r="H496"/>
+          <cell r="I496"/>
+        </row>
+        <row r="497">
+          <cell r="H497"/>
+          <cell r="I497"/>
+        </row>
+        <row r="498">
+          <cell r="H498"/>
+          <cell r="I498"/>
+        </row>
+        <row r="499">
+          <cell r="H499"/>
+          <cell r="I499"/>
+        </row>
+        <row r="500">
+          <cell r="H500"/>
+          <cell r="I500"/>
+        </row>
+        <row r="501">
+          <cell r="H501"/>
+          <cell r="I501"/>
+        </row>
+        <row r="502">
+          <cell r="H502"/>
+          <cell r="I502"/>
+        </row>
+        <row r="503">
+          <cell r="H503"/>
+          <cell r="I503"/>
+        </row>
+        <row r="504">
+          <cell r="H504"/>
+          <cell r="I504"/>
+        </row>
+        <row r="505">
+          <cell r="H505"/>
+          <cell r="I505"/>
+        </row>
+        <row r="506">
+          <cell r="H506"/>
+          <cell r="I506"/>
+        </row>
+        <row r="507">
+          <cell r="H507"/>
+          <cell r="I507"/>
+        </row>
+        <row r="508">
+          <cell r="H508"/>
+          <cell r="I508"/>
+        </row>
+        <row r="509">
+          <cell r="H509"/>
+          <cell r="I509"/>
+        </row>
+        <row r="510">
+          <cell r="H510"/>
+          <cell r="I510"/>
+        </row>
+        <row r="511">
+          <cell r="H511"/>
+          <cell r="I511"/>
+        </row>
+        <row r="512">
+          <cell r="H512"/>
+          <cell r="I512"/>
+        </row>
+        <row r="513">
+          <cell r="H513"/>
+          <cell r="I513"/>
+        </row>
+        <row r="514">
+          <cell r="H514"/>
+          <cell r="I514"/>
+        </row>
+        <row r="515">
+          <cell r="H515"/>
+          <cell r="I515"/>
+        </row>
+        <row r="516">
+          <cell r="H516"/>
+          <cell r="I516"/>
+        </row>
+        <row r="517">
+          <cell r="H517"/>
+          <cell r="I517"/>
+        </row>
+        <row r="518">
+          <cell r="H518"/>
+          <cell r="I518"/>
+        </row>
+        <row r="519">
+          <cell r="H519"/>
+          <cell r="I519"/>
+        </row>
+        <row r="520">
+          <cell r="H520"/>
+          <cell r="I520"/>
+        </row>
+        <row r="521">
+          <cell r="H521"/>
+          <cell r="I521"/>
+        </row>
+        <row r="522">
+          <cell r="H522"/>
+          <cell r="I522"/>
+        </row>
+        <row r="523">
+          <cell r="H523"/>
+          <cell r="I523"/>
+        </row>
+        <row r="524">
+          <cell r="H524"/>
+          <cell r="I524"/>
+        </row>
+        <row r="525">
+          <cell r="H525"/>
+          <cell r="I525"/>
+        </row>
+        <row r="526">
+          <cell r="H526"/>
+          <cell r="I526"/>
+        </row>
+        <row r="527">
+          <cell r="H527"/>
+          <cell r="I527"/>
+        </row>
+        <row r="528">
+          <cell r="H528"/>
+          <cell r="I528"/>
+        </row>
+        <row r="529">
+          <cell r="H529"/>
+          <cell r="I529"/>
+        </row>
+        <row r="530">
+          <cell r="H530"/>
+          <cell r="I530"/>
+        </row>
+        <row r="531">
+          <cell r="H531"/>
+          <cell r="I531"/>
+        </row>
+        <row r="532">
+          <cell r="H532"/>
+          <cell r="I532"/>
+        </row>
+        <row r="533">
+          <cell r="H533"/>
+          <cell r="I533"/>
+        </row>
+        <row r="534">
+          <cell r="H534"/>
+          <cell r="I534"/>
+        </row>
+        <row r="535">
+          <cell r="H535"/>
+          <cell r="I535"/>
+        </row>
+        <row r="536">
+          <cell r="H536"/>
+          <cell r="I536"/>
+        </row>
+        <row r="537">
+          <cell r="H537"/>
+          <cell r="I537"/>
+        </row>
+        <row r="538">
+          <cell r="H538"/>
+          <cell r="I538"/>
+        </row>
+        <row r="539">
+          <cell r="H539"/>
+          <cell r="I539"/>
+        </row>
+        <row r="540">
+          <cell r="H540"/>
+          <cell r="I540"/>
+        </row>
+        <row r="541">
+          <cell r="H541"/>
+          <cell r="I541"/>
+        </row>
+        <row r="542">
+          <cell r="H542"/>
+          <cell r="I542"/>
+        </row>
+        <row r="543">
+          <cell r="H543"/>
+          <cell r="I543"/>
+        </row>
+        <row r="544">
+          <cell r="H544"/>
+          <cell r="I544"/>
+        </row>
+        <row r="545">
+          <cell r="H545"/>
+          <cell r="I545"/>
+        </row>
+        <row r="546">
+          <cell r="H546"/>
+          <cell r="I546"/>
+        </row>
+        <row r="547">
+          <cell r="H547"/>
+          <cell r="I547"/>
+        </row>
+        <row r="548">
+          <cell r="H548"/>
+          <cell r="I548"/>
+        </row>
+        <row r="549">
+          <cell r="H549"/>
+          <cell r="I549"/>
+        </row>
+        <row r="550">
+          <cell r="H550"/>
+          <cell r="I550"/>
+        </row>
+        <row r="551">
+          <cell r="H551"/>
+          <cell r="I551"/>
+        </row>
+        <row r="552">
+          <cell r="H552"/>
+          <cell r="I552"/>
+        </row>
+        <row r="553">
+          <cell r="H553"/>
+          <cell r="I553"/>
+        </row>
+        <row r="554">
+          <cell r="H554"/>
+          <cell r="I554"/>
+        </row>
+        <row r="555">
+          <cell r="H555"/>
+          <cell r="I555"/>
+        </row>
+        <row r="556">
+          <cell r="H556"/>
+          <cell r="I556"/>
+        </row>
+        <row r="557">
+          <cell r="H557"/>
+          <cell r="I557"/>
+        </row>
+        <row r="558">
+          <cell r="H558"/>
+          <cell r="I558"/>
+        </row>
+        <row r="559">
+          <cell r="H559"/>
+          <cell r="I559"/>
+        </row>
+        <row r="560">
+          <cell r="H560"/>
+          <cell r="I560"/>
+        </row>
+        <row r="561">
+          <cell r="H561"/>
+          <cell r="I561"/>
+        </row>
+        <row r="562">
+          <cell r="H562"/>
+          <cell r="I562"/>
+        </row>
+        <row r="563">
+          <cell r="H563"/>
+          <cell r="I563"/>
+        </row>
+        <row r="564">
+          <cell r="H564"/>
+          <cell r="I564"/>
+        </row>
+        <row r="565">
+          <cell r="H565"/>
+          <cell r="I565"/>
+        </row>
+        <row r="566">
+          <cell r="H566"/>
+          <cell r="I566"/>
+        </row>
+        <row r="567">
+          <cell r="H567"/>
+          <cell r="I567"/>
+        </row>
+        <row r="568">
+          <cell r="H568"/>
+          <cell r="I568"/>
+        </row>
+        <row r="569">
+          <cell r="H569"/>
+          <cell r="I569"/>
+        </row>
+        <row r="570">
+          <cell r="H570"/>
+          <cell r="I570"/>
+        </row>
+        <row r="571">
+          <cell r="H571"/>
+          <cell r="I571"/>
+        </row>
+        <row r="572">
+          <cell r="H572"/>
+          <cell r="I572"/>
+        </row>
+        <row r="573">
+          <cell r="H573"/>
+          <cell r="I573"/>
+        </row>
+        <row r="574">
+          <cell r="H574"/>
+          <cell r="I574"/>
+        </row>
+        <row r="575">
+          <cell r="H575"/>
+          <cell r="I575"/>
+        </row>
+        <row r="576">
+          <cell r="H576"/>
+          <cell r="I576"/>
+        </row>
+        <row r="577">
+          <cell r="H577"/>
+          <cell r="I577"/>
+        </row>
+        <row r="578">
+          <cell r="H578"/>
+          <cell r="I578"/>
+        </row>
+        <row r="579">
+          <cell r="H579"/>
+          <cell r="I579"/>
+        </row>
+        <row r="580">
+          <cell r="H580"/>
+          <cell r="I580"/>
+        </row>
+        <row r="581">
+          <cell r="H581"/>
+          <cell r="I581"/>
+        </row>
+        <row r="582">
+          <cell r="H582"/>
+          <cell r="I582"/>
+        </row>
+        <row r="583">
+          <cell r="H583"/>
+          <cell r="I583"/>
+        </row>
+        <row r="584">
+          <cell r="H584"/>
+          <cell r="I584"/>
+        </row>
+        <row r="585">
+          <cell r="H585"/>
+          <cell r="I585"/>
+        </row>
+        <row r="586">
+          <cell r="H586"/>
+          <cell r="I586"/>
+        </row>
+        <row r="587">
+          <cell r="H587"/>
+          <cell r="I587"/>
+        </row>
+        <row r="588">
+          <cell r="H588"/>
+          <cell r="I588"/>
+        </row>
+        <row r="589">
+          <cell r="H589"/>
+          <cell r="I589"/>
+        </row>
+        <row r="590">
+          <cell r="H590"/>
+          <cell r="I590"/>
+        </row>
+        <row r="591">
+          <cell r="H591"/>
+          <cell r="I591"/>
+        </row>
+        <row r="592">
+          <cell r="H592"/>
+          <cell r="I592"/>
+        </row>
+        <row r="593">
+          <cell r="H593"/>
+          <cell r="I593"/>
+        </row>
+        <row r="594">
+          <cell r="H594"/>
+          <cell r="I594"/>
+        </row>
+        <row r="595">
+          <cell r="H595"/>
+          <cell r="I595"/>
+        </row>
+        <row r="596">
+          <cell r="H596"/>
+          <cell r="I596"/>
+        </row>
+        <row r="597">
+          <cell r="H597"/>
+          <cell r="I597"/>
+        </row>
+        <row r="598">
+          <cell r="H598"/>
+          <cell r="I598"/>
+        </row>
+        <row r="599">
+          <cell r="H599"/>
+          <cell r="I599"/>
+        </row>
+        <row r="600">
+          <cell r="H600"/>
+          <cell r="I600"/>
+        </row>
+        <row r="601">
+          <cell r="H601"/>
+          <cell r="I601"/>
+        </row>
+        <row r="602">
+          <cell r="H602"/>
+          <cell r="I602"/>
+        </row>
+        <row r="603">
+          <cell r="H603"/>
+          <cell r="I603"/>
+        </row>
+        <row r="604">
+          <cell r="H604"/>
+          <cell r="I604"/>
+        </row>
+        <row r="605">
+          <cell r="H605"/>
+          <cell r="I605"/>
+        </row>
+        <row r="606">
+          <cell r="H606"/>
+          <cell r="I606"/>
+        </row>
+        <row r="607">
+          <cell r="H607"/>
+          <cell r="I607"/>
+        </row>
+        <row r="608">
+          <cell r="H608"/>
+          <cell r="I608"/>
+        </row>
+        <row r="609">
+          <cell r="H609"/>
+          <cell r="I609"/>
+        </row>
+        <row r="610">
+          <cell r="H610"/>
+          <cell r="I610"/>
+        </row>
+        <row r="611">
+          <cell r="H611"/>
+          <cell r="I611"/>
+        </row>
+        <row r="612">
+          <cell r="H612"/>
+          <cell r="I612"/>
+        </row>
+        <row r="613">
+          <cell r="H613"/>
+          <cell r="I613"/>
+        </row>
+        <row r="614">
+          <cell r="H614"/>
+          <cell r="I614"/>
+        </row>
+        <row r="615">
+          <cell r="H615"/>
+          <cell r="I615"/>
+        </row>
+        <row r="616">
+          <cell r="H616"/>
+          <cell r="I616"/>
+        </row>
+        <row r="617">
+          <cell r="H617"/>
+          <cell r="I617"/>
+        </row>
+        <row r="618">
+          <cell r="H618"/>
+          <cell r="I618"/>
+        </row>
+        <row r="619">
+          <cell r="H619"/>
+          <cell r="I619"/>
+        </row>
+        <row r="620">
+          <cell r="H620"/>
+          <cell r="I620"/>
+        </row>
+        <row r="621">
+          <cell r="H621"/>
+          <cell r="I621"/>
+        </row>
+        <row r="622">
+          <cell r="H622"/>
+          <cell r="I622"/>
+        </row>
+        <row r="623">
+          <cell r="H623"/>
+          <cell r="I623"/>
+        </row>
+        <row r="624">
+          <cell r="H624"/>
+          <cell r="I624"/>
+        </row>
+        <row r="625">
+          <cell r="H625"/>
+          <cell r="I625"/>
+        </row>
+        <row r="626">
+          <cell r="H626"/>
+          <cell r="I626"/>
+        </row>
+        <row r="627">
+          <cell r="H627"/>
+          <cell r="I627"/>
+        </row>
+        <row r="628">
+          <cell r="H628"/>
+          <cell r="I628"/>
+        </row>
+        <row r="629">
+          <cell r="H629"/>
+          <cell r="I629"/>
+        </row>
+        <row r="630">
+          <cell r="H630"/>
+          <cell r="I630"/>
+        </row>
+        <row r="631">
+          <cell r="H631"/>
+          <cell r="I631"/>
+        </row>
+        <row r="632">
+          <cell r="H632"/>
+          <cell r="I632"/>
+        </row>
+        <row r="633">
+          <cell r="H633"/>
+          <cell r="I633"/>
+        </row>
+        <row r="634">
+          <cell r="H634"/>
+          <cell r="I634"/>
+        </row>
+        <row r="635">
+          <cell r="H635"/>
+          <cell r="I635"/>
+        </row>
+        <row r="636">
+          <cell r="H636"/>
+          <cell r="I636"/>
+        </row>
+        <row r="637">
+          <cell r="H637"/>
+          <cell r="I637"/>
+        </row>
+        <row r="638">
+          <cell r="H638"/>
+          <cell r="I638"/>
+        </row>
+        <row r="639">
+          <cell r="H639"/>
+          <cell r="I639"/>
+        </row>
+        <row r="640">
+          <cell r="H640"/>
+          <cell r="I640"/>
+        </row>
+        <row r="641">
+          <cell r="H641"/>
+          <cell r="I641"/>
+        </row>
+        <row r="642">
+          <cell r="H642"/>
+          <cell r="I642"/>
+        </row>
+        <row r="643">
+          <cell r="H643"/>
+          <cell r="I643"/>
+        </row>
+        <row r="644">
+          <cell r="H644"/>
+          <cell r="I644"/>
+        </row>
+        <row r="645">
+          <cell r="H645"/>
+          <cell r="I645"/>
+        </row>
+        <row r="646">
+          <cell r="H646"/>
+          <cell r="I646"/>
+        </row>
+        <row r="647">
+          <cell r="H647"/>
+          <cell r="I647"/>
+        </row>
+        <row r="648">
+          <cell r="H648"/>
+          <cell r="I648"/>
+        </row>
+        <row r="649">
+          <cell r="H649"/>
+          <cell r="I649"/>
+        </row>
+        <row r="650">
+          <cell r="H650"/>
+          <cell r="I650"/>
+        </row>
+        <row r="651">
+          <cell r="H651"/>
+          <cell r="I651"/>
+        </row>
+        <row r="652">
+          <cell r="H652"/>
+          <cell r="I652"/>
+        </row>
+        <row r="653">
+          <cell r="H653"/>
+          <cell r="I653"/>
+        </row>
+        <row r="654">
+          <cell r="H654"/>
+          <cell r="I654"/>
+        </row>
+        <row r="655">
+          <cell r="H655"/>
+          <cell r="I655"/>
+        </row>
+        <row r="656">
+          <cell r="H656"/>
+          <cell r="I656"/>
+        </row>
+        <row r="657">
+          <cell r="H657"/>
+          <cell r="I657"/>
+        </row>
+        <row r="658">
+          <cell r="H658"/>
+          <cell r="I658"/>
+        </row>
+        <row r="659">
+          <cell r="H659"/>
+          <cell r="I659"/>
+        </row>
+        <row r="660">
+          <cell r="H660"/>
+          <cell r="I660"/>
+        </row>
+        <row r="661">
+          <cell r="H661"/>
+          <cell r="I661"/>
+        </row>
+        <row r="662">
+          <cell r="H662"/>
+          <cell r="I662"/>
+        </row>
+        <row r="663">
+          <cell r="H663"/>
+          <cell r="I663"/>
+        </row>
+        <row r="664">
+          <cell r="H664"/>
+          <cell r="I664"/>
+        </row>
+        <row r="665">
+          <cell r="H665"/>
+          <cell r="I665"/>
+        </row>
+        <row r="666">
+          <cell r="H666"/>
+          <cell r="I666"/>
+        </row>
+        <row r="667">
+          <cell r="H667"/>
+          <cell r="I667"/>
+        </row>
+        <row r="668">
+          <cell r="H668"/>
+          <cell r="I668"/>
+        </row>
+        <row r="669">
+          <cell r="H669"/>
+          <cell r="I669"/>
+        </row>
+        <row r="670">
+          <cell r="H670"/>
+          <cell r="I670"/>
+        </row>
+        <row r="671">
+          <cell r="H671"/>
+          <cell r="I671"/>
+        </row>
+        <row r="672">
+          <cell r="H672"/>
+          <cell r="I672"/>
+        </row>
+        <row r="673">
+          <cell r="H673"/>
+          <cell r="I673"/>
+        </row>
+        <row r="674">
+          <cell r="H674"/>
+          <cell r="I674"/>
+        </row>
+        <row r="675">
+          <cell r="H675"/>
+          <cell r="I675"/>
+        </row>
+        <row r="676">
+          <cell r="H676"/>
+          <cell r="I676"/>
+        </row>
+        <row r="677">
+          <cell r="H677"/>
+          <cell r="I677"/>
+        </row>
+        <row r="678">
+          <cell r="H678"/>
+          <cell r="I678"/>
+        </row>
+        <row r="679">
+          <cell r="H679"/>
+          <cell r="I679"/>
+        </row>
+        <row r="680">
+          <cell r="H680"/>
+          <cell r="I680"/>
+        </row>
+        <row r="681">
+          <cell r="H681"/>
+          <cell r="I681"/>
+        </row>
+        <row r="682">
+          <cell r="H682"/>
+          <cell r="I682"/>
+        </row>
+        <row r="683">
+          <cell r="H683"/>
+          <cell r="I683"/>
+        </row>
+        <row r="684">
+          <cell r="H684"/>
+          <cell r="I684"/>
+        </row>
+        <row r="685">
+          <cell r="H685"/>
+          <cell r="I685"/>
+        </row>
+        <row r="686">
+          <cell r="H686"/>
+          <cell r="I686"/>
+        </row>
+        <row r="687">
+          <cell r="H687"/>
+          <cell r="I687"/>
+        </row>
+        <row r="688">
+          <cell r="H688"/>
+          <cell r="I688"/>
+        </row>
+        <row r="689">
+          <cell r="H689"/>
+          <cell r="I689"/>
+        </row>
+        <row r="690">
+          <cell r="H690"/>
+          <cell r="I690"/>
+        </row>
+        <row r="691">
+          <cell r="H691"/>
+          <cell r="I691"/>
+        </row>
+        <row r="692">
+          <cell r="H692"/>
+          <cell r="I692"/>
+        </row>
+        <row r="693">
+          <cell r="H693"/>
+          <cell r="I693"/>
+        </row>
+        <row r="694">
+          <cell r="H694"/>
+          <cell r="I694"/>
+        </row>
+        <row r="695">
+          <cell r="H695"/>
+          <cell r="I695"/>
+        </row>
+        <row r="696">
+          <cell r="H696"/>
+          <cell r="I696"/>
+        </row>
+        <row r="697">
+          <cell r="H697"/>
+          <cell r="I697"/>
+        </row>
+        <row r="698">
+          <cell r="H698"/>
+          <cell r="I698"/>
+        </row>
+        <row r="699">
+          <cell r="H699"/>
+          <cell r="I699"/>
+        </row>
+        <row r="700">
+          <cell r="H700"/>
+          <cell r="I700"/>
+        </row>
+        <row r="701">
+          <cell r="H701"/>
+          <cell r="I701"/>
+        </row>
+        <row r="702">
+          <cell r="H702"/>
+          <cell r="I702"/>
+        </row>
+        <row r="703">
+          <cell r="H703"/>
+          <cell r="I703"/>
+        </row>
+        <row r="704">
+          <cell r="H704"/>
+          <cell r="I704"/>
+        </row>
+        <row r="705">
+          <cell r="H705"/>
+          <cell r="I705"/>
+        </row>
+        <row r="706">
+          <cell r="H706"/>
+          <cell r="I706"/>
+        </row>
+        <row r="707">
+          <cell r="H707"/>
+          <cell r="I707"/>
+        </row>
+        <row r="708">
+          <cell r="H708"/>
+          <cell r="I708"/>
+        </row>
+        <row r="709">
+          <cell r="H709"/>
+          <cell r="I709"/>
+        </row>
+        <row r="710">
+          <cell r="H710"/>
+          <cell r="I710"/>
+        </row>
+        <row r="711">
+          <cell r="H711"/>
+          <cell r="I711"/>
+        </row>
+        <row r="712">
+          <cell r="H712"/>
+          <cell r="I712"/>
+        </row>
+        <row r="713">
+          <cell r="H713"/>
+          <cell r="I713"/>
+        </row>
+        <row r="714">
+          <cell r="H714"/>
+          <cell r="I714"/>
+        </row>
+        <row r="715">
+          <cell r="H715"/>
+          <cell r="I715"/>
+        </row>
+        <row r="716">
+          <cell r="H716"/>
+          <cell r="I716"/>
+        </row>
+        <row r="717">
+          <cell r="H717"/>
+          <cell r="I717"/>
+        </row>
+        <row r="718">
+          <cell r="H718"/>
+          <cell r="I718"/>
+        </row>
+        <row r="719">
+          <cell r="H719"/>
+          <cell r="I719"/>
+        </row>
+        <row r="720">
+          <cell r="H720"/>
+          <cell r="I720"/>
+        </row>
+        <row r="721">
+          <cell r="H721"/>
+          <cell r="I721"/>
+        </row>
+        <row r="722">
+          <cell r="H722"/>
+          <cell r="I722"/>
+        </row>
+        <row r="723">
+          <cell r="H723"/>
+          <cell r="I723"/>
+        </row>
+        <row r="724">
+          <cell r="H724"/>
+          <cell r="I724"/>
+        </row>
+        <row r="725">
+          <cell r="H725"/>
+          <cell r="I725"/>
+        </row>
+        <row r="726">
+          <cell r="H726"/>
+          <cell r="I726"/>
+        </row>
+        <row r="727">
+          <cell r="H727"/>
+          <cell r="I727"/>
+        </row>
+        <row r="728">
+          <cell r="H728"/>
+          <cell r="I728"/>
+        </row>
+        <row r="729">
+          <cell r="H729"/>
+          <cell r="I729"/>
+        </row>
+        <row r="730">
+          <cell r="H730"/>
+          <cell r="I730"/>
+        </row>
+        <row r="731">
+          <cell r="H731"/>
+          <cell r="I731"/>
+        </row>
+        <row r="732">
+          <cell r="H732"/>
+          <cell r="I732"/>
+        </row>
+        <row r="733">
+          <cell r="H733"/>
+          <cell r="I733"/>
+        </row>
+        <row r="734">
+          <cell r="H734"/>
+          <cell r="I734"/>
+        </row>
+        <row r="735">
+          <cell r="H735"/>
+          <cell r="I735"/>
+        </row>
+        <row r="736">
+          <cell r="H736"/>
+          <cell r="I736"/>
+        </row>
+        <row r="737">
+          <cell r="H737"/>
+          <cell r="I737"/>
+        </row>
+        <row r="738">
+          <cell r="H738"/>
+          <cell r="I738"/>
+        </row>
+        <row r="739">
+          <cell r="H739"/>
+          <cell r="I739"/>
+        </row>
+        <row r="740">
+          <cell r="H740"/>
+          <cell r="I740"/>
+        </row>
+        <row r="741">
+          <cell r="H741"/>
+          <cell r="I741"/>
+        </row>
+        <row r="742">
+          <cell r="H742"/>
+          <cell r="I742"/>
+        </row>
+        <row r="743">
+          <cell r="H743"/>
+          <cell r="I743"/>
+        </row>
+        <row r="744">
+          <cell r="H744"/>
+          <cell r="I744"/>
+        </row>
+        <row r="745">
+          <cell r="H745"/>
+          <cell r="I745"/>
+        </row>
+        <row r="746">
+          <cell r="H746"/>
+          <cell r="I746"/>
+        </row>
+        <row r="747">
+          <cell r="H747"/>
+          <cell r="I747"/>
+        </row>
+        <row r="748">
+          <cell r="H748"/>
+          <cell r="I748"/>
+        </row>
+        <row r="749">
+          <cell r="H749"/>
+          <cell r="I749"/>
+        </row>
+        <row r="750">
+          <cell r="H750"/>
+          <cell r="I750"/>
+        </row>
+        <row r="751">
+          <cell r="H751"/>
+          <cell r="I751"/>
+        </row>
+        <row r="752">
+          <cell r="H752"/>
+          <cell r="I752"/>
+        </row>
+        <row r="753">
+          <cell r="H753"/>
+          <cell r="I753"/>
+        </row>
+        <row r="754">
+          <cell r="H754"/>
+          <cell r="I754"/>
+        </row>
+        <row r="755">
+          <cell r="H755"/>
+          <cell r="I755"/>
+        </row>
+        <row r="756">
+          <cell r="H756"/>
+          <cell r="I756"/>
+        </row>
+        <row r="757">
+          <cell r="H757"/>
+          <cell r="I757"/>
+        </row>
+        <row r="758">
+          <cell r="H758"/>
+          <cell r="I758"/>
+        </row>
+        <row r="759">
+          <cell r="H759"/>
+          <cell r="I759"/>
+        </row>
+        <row r="760">
+          <cell r="H760"/>
+          <cell r="I760"/>
+        </row>
+        <row r="761">
+          <cell r="H761"/>
+          <cell r="I761"/>
+        </row>
+        <row r="762">
+          <cell r="H762"/>
+          <cell r="I762"/>
+        </row>
+        <row r="763">
+          <cell r="H763"/>
+          <cell r="I763"/>
+        </row>
+        <row r="764">
+          <cell r="H764"/>
+          <cell r="I764"/>
+        </row>
+        <row r="765">
+          <cell r="H765"/>
+          <cell r="I765"/>
+        </row>
+        <row r="766">
+          <cell r="H766"/>
+          <cell r="I766"/>
+        </row>
+        <row r="767">
+          <cell r="H767"/>
+          <cell r="I767"/>
+        </row>
+        <row r="768">
+          <cell r="H768"/>
+          <cell r="I768"/>
+        </row>
+        <row r="769">
+          <cell r="H769"/>
+          <cell r="I769"/>
+        </row>
+        <row r="770">
+          <cell r="H770"/>
+          <cell r="I770"/>
+        </row>
+        <row r="771">
+          <cell r="H771"/>
+          <cell r="I771"/>
+        </row>
+        <row r="772">
+          <cell r="H772"/>
+          <cell r="I772"/>
+        </row>
+        <row r="773">
+          <cell r="H773"/>
+          <cell r="I773"/>
+        </row>
+        <row r="774">
+          <cell r="H774"/>
+          <cell r="I774"/>
+        </row>
+        <row r="775">
+          <cell r="H775"/>
+          <cell r="I775"/>
+        </row>
+        <row r="776">
+          <cell r="H776"/>
+          <cell r="I776"/>
+        </row>
+        <row r="777">
+          <cell r="H777"/>
+          <cell r="I777"/>
+        </row>
+        <row r="778">
+          <cell r="H778"/>
+          <cell r="I778"/>
+        </row>
+        <row r="779">
+          <cell r="H779"/>
+          <cell r="I779"/>
+        </row>
+        <row r="780">
+          <cell r="H780"/>
+          <cell r="I780"/>
+        </row>
+        <row r="781">
+          <cell r="H781"/>
+          <cell r="I781"/>
+        </row>
+        <row r="782">
+          <cell r="H782"/>
+          <cell r="I782"/>
+        </row>
+        <row r="783">
+          <cell r="H783"/>
+          <cell r="I783"/>
+        </row>
+        <row r="784">
+          <cell r="H784"/>
+          <cell r="I784"/>
+        </row>
+        <row r="785">
+          <cell r="H785"/>
+          <cell r="I785"/>
+        </row>
+        <row r="786">
+          <cell r="H786"/>
+          <cell r="I786"/>
+        </row>
+        <row r="787">
+          <cell r="H787"/>
+          <cell r="I787"/>
+        </row>
+        <row r="788">
+          <cell r="H788"/>
+          <cell r="I788"/>
+        </row>
+        <row r="789">
+          <cell r="H789"/>
+          <cell r="I789"/>
+        </row>
+        <row r="790">
+          <cell r="H790"/>
+          <cell r="I790"/>
+        </row>
+        <row r="791">
+          <cell r="H791"/>
+          <cell r="I791"/>
+        </row>
+        <row r="792">
+          <cell r="H792"/>
+          <cell r="I792"/>
+        </row>
+        <row r="793">
+          <cell r="H793"/>
+          <cell r="I793"/>
+        </row>
+        <row r="794">
+          <cell r="H794"/>
+          <cell r="I794"/>
+        </row>
+        <row r="795">
+          <cell r="H795"/>
+          <cell r="I795"/>
+        </row>
+        <row r="796">
+          <cell r="H796"/>
+          <cell r="I796"/>
+        </row>
+        <row r="797">
+          <cell r="H797"/>
+          <cell r="I797"/>
+        </row>
+        <row r="798">
+          <cell r="H798"/>
+          <cell r="I798"/>
+        </row>
+        <row r="799">
+          <cell r="H799"/>
+          <cell r="I799"/>
+        </row>
+        <row r="800">
+          <cell r="H800"/>
+          <cell r="I800"/>
+        </row>
+        <row r="801">
+          <cell r="H801"/>
+          <cell r="I801"/>
+        </row>
+        <row r="802">
+          <cell r="H802"/>
+          <cell r="I802"/>
+        </row>
+        <row r="803">
+          <cell r="H803"/>
+          <cell r="I803"/>
+        </row>
+        <row r="804">
+          <cell r="H804"/>
+          <cell r="I804"/>
+        </row>
+        <row r="805">
+          <cell r="H805"/>
+          <cell r="I805"/>
+        </row>
+        <row r="806">
+          <cell r="H806"/>
+          <cell r="I806"/>
+        </row>
+        <row r="807">
+          <cell r="H807"/>
+          <cell r="I807"/>
+        </row>
+        <row r="808">
+          <cell r="H808"/>
+          <cell r="I808"/>
+        </row>
+        <row r="809">
+          <cell r="H809"/>
+          <cell r="I809"/>
+        </row>
+        <row r="810">
+          <cell r="H810"/>
+          <cell r="I810"/>
+        </row>
+        <row r="811">
+          <cell r="H811"/>
+          <cell r="I811"/>
+        </row>
+        <row r="812">
+          <cell r="H812"/>
+          <cell r="I812"/>
+        </row>
+        <row r="813">
+          <cell r="H813"/>
+          <cell r="I813"/>
+        </row>
+        <row r="814">
+          <cell r="H814"/>
+          <cell r="I814"/>
+        </row>
+        <row r="815">
+          <cell r="H815"/>
+          <cell r="I815"/>
+        </row>
+        <row r="816">
+          <cell r="H816"/>
+          <cell r="I816"/>
+        </row>
+        <row r="817">
+          <cell r="H817"/>
+          <cell r="I817"/>
+        </row>
+        <row r="818">
+          <cell r="H818"/>
+          <cell r="I818"/>
+        </row>
+        <row r="819">
+          <cell r="H819"/>
+          <cell r="I819"/>
+        </row>
+        <row r="820">
+          <cell r="H820"/>
+          <cell r="I820"/>
+        </row>
+        <row r="821">
+          <cell r="H821"/>
+          <cell r="I821"/>
+        </row>
+        <row r="822">
+          <cell r="H822"/>
+          <cell r="I822"/>
+        </row>
+        <row r="823">
+          <cell r="H823"/>
+          <cell r="I823"/>
+        </row>
+        <row r="824">
+          <cell r="H824"/>
+          <cell r="I824"/>
+        </row>
+        <row r="825">
+          <cell r="H825"/>
+          <cell r="I825"/>
+        </row>
+        <row r="826">
+          <cell r="H826"/>
+          <cell r="I826"/>
+        </row>
+        <row r="827">
+          <cell r="H827"/>
+          <cell r="I827"/>
+        </row>
+        <row r="828">
+          <cell r="H828"/>
+          <cell r="I828"/>
+        </row>
+        <row r="829">
+          <cell r="H829"/>
+          <cell r="I829"/>
+        </row>
+        <row r="830">
+          <cell r="H830"/>
+          <cell r="I830"/>
+        </row>
+        <row r="831">
+          <cell r="H831"/>
+          <cell r="I831"/>
+        </row>
+        <row r="832">
+          <cell r="H832"/>
+          <cell r="I832"/>
+        </row>
+        <row r="833">
+          <cell r="H833"/>
+          <cell r="I833"/>
+        </row>
+        <row r="834">
+          <cell r="H834"/>
+          <cell r="I834"/>
+        </row>
+        <row r="835">
+          <cell r="H835"/>
+          <cell r="I835"/>
+        </row>
+        <row r="836">
+          <cell r="H836"/>
+          <cell r="I836"/>
+        </row>
+        <row r="837">
+          <cell r="H837"/>
+          <cell r="I837"/>
+        </row>
+        <row r="838">
+          <cell r="H838"/>
+          <cell r="I838"/>
+        </row>
+        <row r="839">
+          <cell r="H839"/>
+          <cell r="I839"/>
+        </row>
+        <row r="840">
+          <cell r="H840"/>
+          <cell r="I840"/>
+        </row>
+        <row r="841">
+          <cell r="H841"/>
+          <cell r="I841"/>
+        </row>
+        <row r="842">
+          <cell r="H842"/>
+          <cell r="I842"/>
+        </row>
+        <row r="843">
+          <cell r="H843"/>
+          <cell r="I843"/>
+        </row>
+        <row r="844">
+          <cell r="H844"/>
+          <cell r="I844"/>
+        </row>
+        <row r="845">
+          <cell r="H845"/>
+          <cell r="I845"/>
+        </row>
+        <row r="846">
+          <cell r="H846"/>
+          <cell r="I846"/>
+        </row>
+        <row r="847">
+          <cell r="H847"/>
+          <cell r="I847"/>
+        </row>
+        <row r="848">
+          <cell r="H848"/>
+          <cell r="I848"/>
+        </row>
+        <row r="849">
+          <cell r="H849"/>
+          <cell r="I849"/>
+        </row>
+        <row r="850">
+          <cell r="H850"/>
+          <cell r="I850"/>
+        </row>
+        <row r="851">
+          <cell r="H851"/>
+          <cell r="I851"/>
+        </row>
+        <row r="852">
+          <cell r="H852"/>
+          <cell r="I852"/>
+        </row>
+        <row r="853">
+          <cell r="H853"/>
+          <cell r="I853"/>
+        </row>
+        <row r="854">
+          <cell r="H854"/>
+          <cell r="I854"/>
+        </row>
+        <row r="855">
+          <cell r="H855"/>
+          <cell r="I855"/>
+        </row>
+        <row r="856">
+          <cell r="H856"/>
+          <cell r="I856"/>
+        </row>
+        <row r="857">
+          <cell r="H857"/>
+          <cell r="I857"/>
+        </row>
+        <row r="858">
+          <cell r="H858"/>
+          <cell r="I858"/>
+        </row>
+        <row r="859">
+          <cell r="H859"/>
+          <cell r="I859"/>
+        </row>
+        <row r="860">
+          <cell r="H860"/>
+          <cell r="I860"/>
+        </row>
+        <row r="861">
+          <cell r="H861"/>
+          <cell r="I861"/>
+        </row>
+        <row r="862">
+          <cell r="H862"/>
+          <cell r="I862"/>
+        </row>
+        <row r="863">
+          <cell r="H863"/>
+          <cell r="I863"/>
+        </row>
+        <row r="864">
+          <cell r="H864"/>
+          <cell r="I864"/>
+        </row>
+        <row r="865">
+          <cell r="H865"/>
+          <cell r="I865"/>
+        </row>
+        <row r="866">
+          <cell r="H866"/>
+          <cell r="I866"/>
+        </row>
+        <row r="867">
+          <cell r="H867"/>
+          <cell r="I867"/>
+        </row>
+        <row r="868">
+          <cell r="H868"/>
+          <cell r="I868"/>
+        </row>
+        <row r="869">
+          <cell r="H869"/>
+          <cell r="I869"/>
+        </row>
+        <row r="870">
+          <cell r="H870"/>
+          <cell r="I870"/>
+        </row>
+        <row r="871">
+          <cell r="H871"/>
+          <cell r="I871"/>
+        </row>
+        <row r="872">
+          <cell r="H872"/>
+          <cell r="I872"/>
+        </row>
+        <row r="873">
+          <cell r="H873"/>
+          <cell r="I873"/>
+        </row>
+        <row r="874">
+          <cell r="H874"/>
+          <cell r="I874"/>
+        </row>
+        <row r="875">
+          <cell r="H875"/>
+          <cell r="I875"/>
+        </row>
+        <row r="876">
+          <cell r="H876"/>
+          <cell r="I876"/>
+        </row>
+        <row r="877">
+          <cell r="H877"/>
+          <cell r="I877"/>
+        </row>
+        <row r="878">
+          <cell r="H878"/>
+          <cell r="I878"/>
+        </row>
+        <row r="879">
+          <cell r="H879"/>
+          <cell r="I879"/>
+        </row>
+        <row r="880">
+          <cell r="H880"/>
+          <cell r="I880"/>
+        </row>
+        <row r="881">
+          <cell r="H881"/>
+          <cell r="I881"/>
+        </row>
+        <row r="882">
+          <cell r="H882"/>
+          <cell r="I882"/>
+        </row>
+        <row r="883">
+          <cell r="H883"/>
+          <cell r="I883"/>
+        </row>
+        <row r="884">
+          <cell r="H884"/>
+          <cell r="I884"/>
+        </row>
+        <row r="885">
+          <cell r="H885"/>
+          <cell r="I885"/>
+        </row>
+        <row r="886">
+          <cell r="H886"/>
+          <cell r="I886"/>
+        </row>
+        <row r="887">
+          <cell r="H887"/>
+          <cell r="I887"/>
+        </row>
+        <row r="888">
+          <cell r="H888"/>
+          <cell r="I888"/>
+        </row>
+        <row r="889">
+          <cell r="H889"/>
+          <cell r="I889"/>
+        </row>
+        <row r="890">
+          <cell r="H890"/>
+          <cell r="I890"/>
+        </row>
+        <row r="891">
+          <cell r="H891"/>
+          <cell r="I891"/>
+        </row>
+        <row r="892">
+          <cell r="H892"/>
+          <cell r="I892"/>
+        </row>
+        <row r="893">
+          <cell r="H893"/>
+          <cell r="I893"/>
+        </row>
+        <row r="894">
+          <cell r="H894"/>
+          <cell r="I894"/>
+        </row>
+        <row r="895">
+          <cell r="H895"/>
+          <cell r="I895"/>
+        </row>
+        <row r="896">
+          <cell r="H896"/>
+          <cell r="I896"/>
+        </row>
+        <row r="897">
+          <cell r="H897"/>
+          <cell r="I897"/>
+        </row>
+        <row r="898">
+          <cell r="H898"/>
+          <cell r="I898"/>
+        </row>
+        <row r="899">
+          <cell r="H899"/>
+          <cell r="I899"/>
+        </row>
+        <row r="900">
+          <cell r="H900"/>
+          <cell r="I900"/>
+        </row>
+        <row r="901">
+          <cell r="H901"/>
+          <cell r="I901"/>
+        </row>
+        <row r="902">
+          <cell r="H902"/>
+          <cell r="I902"/>
+        </row>
+        <row r="903">
+          <cell r="H903"/>
+          <cell r="I903"/>
+        </row>
+        <row r="904">
+          <cell r="H904"/>
+          <cell r="I904"/>
+        </row>
+        <row r="905">
+          <cell r="H905"/>
+          <cell r="I905"/>
+        </row>
+        <row r="906">
+          <cell r="H906"/>
+          <cell r="I906"/>
+        </row>
+        <row r="907">
+          <cell r="H907"/>
+          <cell r="I907"/>
+        </row>
+        <row r="908">
+          <cell r="H908"/>
+          <cell r="I908"/>
+        </row>
+        <row r="909">
+          <cell r="H909"/>
+          <cell r="I909"/>
+        </row>
+        <row r="910">
+          <cell r="H910"/>
+          <cell r="I910"/>
+        </row>
+        <row r="911">
+          <cell r="H911"/>
+          <cell r="I911"/>
+        </row>
+        <row r="912">
+          <cell r="H912"/>
+          <cell r="I912"/>
+        </row>
+        <row r="913">
+          <cell r="H913"/>
+          <cell r="I913"/>
+        </row>
+        <row r="914">
+          <cell r="H914"/>
+          <cell r="I914"/>
+        </row>
+        <row r="915">
+          <cell r="H915"/>
+          <cell r="I915"/>
+        </row>
+        <row r="916">
+          <cell r="H916"/>
+          <cell r="I916"/>
+        </row>
+        <row r="917">
+          <cell r="H917"/>
+          <cell r="I917"/>
+        </row>
+        <row r="918">
+          <cell r="H918"/>
+          <cell r="I918"/>
+        </row>
+        <row r="919">
+          <cell r="H919"/>
+          <cell r="I919"/>
+        </row>
+        <row r="920">
+          <cell r="H920"/>
+          <cell r="I920"/>
+        </row>
+        <row r="921">
+          <cell r="H921"/>
+          <cell r="I921"/>
+        </row>
+        <row r="922">
+          <cell r="H922"/>
+          <cell r="I922"/>
+        </row>
+        <row r="923">
+          <cell r="H923"/>
+          <cell r="I923"/>
+        </row>
+        <row r="924">
+          <cell r="H924"/>
+          <cell r="I924"/>
+        </row>
+        <row r="925">
+          <cell r="H925"/>
+          <cell r="I925"/>
+        </row>
+        <row r="926">
+          <cell r="H926"/>
+          <cell r="I926"/>
+        </row>
+        <row r="927">
+          <cell r="H927"/>
+          <cell r="I927"/>
+        </row>
+        <row r="928">
+          <cell r="H928"/>
+          <cell r="I928"/>
+        </row>
+        <row r="929">
+          <cell r="H929"/>
+          <cell r="I929"/>
+        </row>
+        <row r="930">
+          <cell r="H930"/>
+          <cell r="I930"/>
+        </row>
+        <row r="931">
+          <cell r="H931"/>
+          <cell r="I931"/>
+        </row>
+        <row r="932">
+          <cell r="H932"/>
+          <cell r="I932"/>
+        </row>
+        <row r="933">
+          <cell r="H933"/>
+          <cell r="I933"/>
+        </row>
+        <row r="934">
+          <cell r="H934"/>
+          <cell r="I934"/>
+        </row>
+        <row r="935">
+          <cell r="H935"/>
+          <cell r="I935"/>
+        </row>
+        <row r="936">
+          <cell r="H936"/>
+          <cell r="I936"/>
+        </row>
+        <row r="937">
+          <cell r="H937"/>
+          <cell r="I937"/>
+        </row>
+        <row r="938">
+          <cell r="H938"/>
+          <cell r="I938"/>
+        </row>
+        <row r="939">
+          <cell r="H939"/>
+          <cell r="I939"/>
+        </row>
+        <row r="940">
+          <cell r="H940"/>
+          <cell r="I940"/>
+        </row>
+        <row r="941">
+          <cell r="H941"/>
+          <cell r="I941"/>
+        </row>
+        <row r="942">
+          <cell r="H942"/>
+          <cell r="I942"/>
+        </row>
+        <row r="943">
+          <cell r="H943"/>
+          <cell r="I943"/>
+        </row>
+        <row r="944">
+          <cell r="H944"/>
+          <cell r="I944"/>
+        </row>
+        <row r="945">
+          <cell r="H945"/>
+          <cell r="I945"/>
+        </row>
+        <row r="946">
+          <cell r="H946"/>
+          <cell r="I946"/>
+        </row>
+        <row r="947">
+          <cell r="H947"/>
+          <cell r="I947"/>
+        </row>
+        <row r="948">
+          <cell r="H948"/>
+          <cell r="I948"/>
+        </row>
+        <row r="949">
+          <cell r="H949"/>
+          <cell r="I949"/>
+        </row>
+        <row r="950">
+          <cell r="H950"/>
+          <cell r="I950"/>
+        </row>
+        <row r="951">
+          <cell r="H951"/>
+          <cell r="I951"/>
+        </row>
+        <row r="952">
+          <cell r="H952"/>
+          <cell r="I952"/>
+        </row>
+        <row r="953">
+          <cell r="H953"/>
+          <cell r="I953"/>
+        </row>
+        <row r="954">
+          <cell r="H954"/>
+          <cell r="I954"/>
+        </row>
+        <row r="955">
+          <cell r="H955"/>
+          <cell r="I955"/>
+        </row>
+        <row r="956">
+          <cell r="H956"/>
+          <cell r="I956"/>
+        </row>
+        <row r="957">
+          <cell r="H957"/>
+          <cell r="I957"/>
+        </row>
+        <row r="958">
+          <cell r="H958"/>
+          <cell r="I958"/>
+        </row>
+        <row r="959">
+          <cell r="H959"/>
+          <cell r="I959"/>
+        </row>
+        <row r="960">
+          <cell r="H960"/>
+          <cell r="I960"/>
+        </row>
+        <row r="961">
+          <cell r="H961"/>
+          <cell r="I961"/>
+        </row>
+        <row r="962">
+          <cell r="H962"/>
+          <cell r="I962"/>
+        </row>
+        <row r="963">
+          <cell r="H963"/>
+          <cell r="I963"/>
+        </row>
+        <row r="964">
+          <cell r="H964"/>
+          <cell r="I964"/>
+        </row>
+        <row r="965">
+          <cell r="H965"/>
+          <cell r="I965"/>
+        </row>
+        <row r="966">
+          <cell r="H966"/>
+          <cell r="I966"/>
+        </row>
+        <row r="967">
+          <cell r="H967"/>
+          <cell r="I967"/>
+        </row>
+        <row r="968">
+          <cell r="H968"/>
+          <cell r="I968"/>
+        </row>
+        <row r="969">
+          <cell r="H969"/>
+          <cell r="I969"/>
+        </row>
+        <row r="970">
+          <cell r="H970"/>
+          <cell r="I970"/>
+        </row>
+        <row r="971">
+          <cell r="H971"/>
+          <cell r="I971"/>
+        </row>
+        <row r="972">
+          <cell r="H972"/>
+          <cell r="I972"/>
+        </row>
+        <row r="973">
+          <cell r="H973"/>
+          <cell r="I973"/>
+        </row>
+        <row r="974">
+          <cell r="H974"/>
+          <cell r="I974"/>
+        </row>
+        <row r="975">
+          <cell r="H975"/>
+          <cell r="I975"/>
+        </row>
+        <row r="976">
+          <cell r="H976"/>
+          <cell r="I976"/>
+        </row>
+        <row r="977">
+          <cell r="H977"/>
+          <cell r="I977"/>
+        </row>
+        <row r="978">
+          <cell r="H978"/>
+          <cell r="I978"/>
+        </row>
+        <row r="979">
+          <cell r="H979"/>
+          <cell r="I979"/>
+        </row>
+        <row r="980">
+          <cell r="H980"/>
+          <cell r="I980"/>
+        </row>
+        <row r="981">
+          <cell r="H981"/>
+          <cell r="I981"/>
+        </row>
+        <row r="982">
+          <cell r="H982"/>
+          <cell r="I982"/>
+        </row>
+        <row r="983">
+          <cell r="H983"/>
+          <cell r="I983"/>
+        </row>
+        <row r="984">
+          <cell r="H984"/>
+          <cell r="I984"/>
+        </row>
+        <row r="985">
+          <cell r="H985"/>
+          <cell r="I985"/>
+        </row>
+        <row r="986">
+          <cell r="H986"/>
+          <cell r="I986"/>
+        </row>
+        <row r="987">
+          <cell r="H987"/>
+          <cell r="I987"/>
+        </row>
+        <row r="988">
+          <cell r="H988"/>
+          <cell r="I988"/>
+        </row>
+        <row r="989">
+          <cell r="H989"/>
+          <cell r="I989"/>
+        </row>
+        <row r="990">
+          <cell r="H990"/>
+          <cell r="I990"/>
+        </row>
+        <row r="991">
+          <cell r="H991"/>
+          <cell r="I991"/>
+        </row>
       </sheetData>
       <sheetData sheetId="14"/>
       <sheetData sheetId="15"/>

</xml_diff>

<commit_message>
Removing unused files and improving metadata info in README
</commit_message>
<xml_diff>
--- a/rawdata/PastureMeterCalibration.xlsx
+++ b/rawdata/PastureMeterCalibration.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elwel\OneDrive\Desktop\AppraisingGrazing\rawdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A6C8420-77C3-491B-A329-90135D87A37F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EF8662E-8203-4702-803C-FCD067C53EFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{529C1CFA-C348-486F-AA08-2F4EEFEEB289}"/>
   </bookViews>
@@ -309,678 +309,6 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.15840269966254217"/>
-          <c:y val="0.2384584342211461"/>
-          <c:w val="0.80454968128983895"/>
-          <c:h val="0.66792466619638646"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>[1]PasterMeterCalibration!$I$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>dry biomass (g)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-0.51241579177602803"/>
-                  <c:y val="-0.30527303878681833"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>[1]PasterMeterCalibration!$H$2:$H$991</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="990"/>
-                <c:pt idx="0">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>39</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>12.5</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>18</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>[1]PasterMeterCalibration!$I$2:$I$991</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="990"/>
-                <c:pt idx="0">
-                  <c:v>51.2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>62.8</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>37.9</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>41.2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7.6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>20.2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>26.6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>22.1</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.1000000000000001</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>13.7</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>51.3</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>22.7</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>16.8</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>42.8</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>25.52</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>218.88</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>24.61</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>23.37</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>18.27</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>133.22</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>61.55</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>61.83</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>52.78</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>55.01</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>133.81</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>79.069999999999993</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>154.16999999999999</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>151.26</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>73.819999999999993</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>77.97</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>50.65</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>50.5</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>48.24</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>85.11</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>99.45</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>77.08</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>41.56</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>87.79</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>62.85</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>110.47</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>61.28</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>103</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>129.38</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>156.99</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>80.510000000000005</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>153.44</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>60.01</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>100.73</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>132.59</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-9E16-4552-967C-7CDD03293333}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="1353530639"/>
-        <c:axId val="1353528559"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="1353530639"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1353528559"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="1353528559"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1353530639"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1663,563 +991,7 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2740,53 +1512,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>586740</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:colOff>845820</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>64770</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>708660</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{380F75C5-BE6B-4C94-93C7-A59CDAECDC17}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>22860</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>251460</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>205740</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>64770</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2805,7 +1539,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -7034,9 +5768,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -7074,7 +5808,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -7180,7 +5914,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -7322,7 +6056,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -7332,8 +6066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{617FA0DB-87D6-48CC-B2AB-36E698C714D8}">
   <dimension ref="A1:I991"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="I1" activeCellId="1" sqref="H1:H1048576 I1:I1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>